<commit_message>
Edits in Bugs File
</commit_message>
<xml_diff>
--- a/TestCases_Bugs/GobusBugs.xlsx
+++ b/TestCases_Bugs/GobusBugs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\GOBUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11E58F8-1561-49C6-9FA2-4E90B29437D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A30028-B62E-4EBE-AA8B-3F54E684723B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{26FBA53E-1270-4504-9D9A-41981D0E1731}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Steps of the Bug</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Screen Shot/Record</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Terms and conditions content is arabic despite of app language is English </t>
   </si>
   <si>
     <t>1-Open GoBus App
@@ -75,18 +72,12 @@
     <t>Medium</t>
   </si>
   <si>
-    <t xml:space="preserve">Read More button in about us screen doesn't work </t>
-  </si>
-  <si>
     <t xml:space="preserve">1-Open GoBus App
 2-Click On More 
 3-Click on About Us 
 4-Click on Read More Button </t>
   </si>
   <si>
-    <t xml:space="preserve">Another content is displayed </t>
-  </si>
-  <si>
     <t>No action</t>
   </si>
   <si>
@@ -105,9 +96,6 @@
     <t>all items are unique</t>
   </si>
   <si>
-    <t>User can't Edit his registred information</t>
-  </si>
-  <si>
     <t xml:space="preserve">1-Open GoBus App 
 2-Click on Account
 3-Create New Account 
@@ -134,9 +122,6 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1VJ2WJUOcLqhEUkqDi7LQ-nBSd2EmDArW/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>User Can't book his Trip</t>
   </si>
   <si>
     <t>1-Open GoBus App 
@@ -161,10 +146,51 @@
     <t>https://drive.google.com/file/d/1Twkz6tcpH-MR3kyVd-aW6gtunDwaCE1c/view?usp=sharing</t>
   </si>
   <si>
-    <t xml:space="preserve">Medium </t>
-  </si>
-  <si>
     <t>blocker</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>minor</t>
+  </si>
+  <si>
+    <t>major</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Major </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Terms and conditions content is writen in Arabic language while device language is English</t>
+  </si>
+  <si>
+    <t>Read More button functionality is not working properly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full content should be displayed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unexpected validation message is displayed when User click on confirm button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No option to edit registered account information </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No option to reset/change password </t>
+  </si>
+  <si>
+    <t>1-Open GoBus App 
+2-Click onlogin with an email
+ 3-Verify change/reset password option is exist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change/Reset password optionis exist </t>
+  </si>
+  <si>
+    <t>No option to change/reset password</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1B3_hRno5PwSfg7HPUI4F1hEg5gMbI0sj/view?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -567,10 +593,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097A79EB-57C5-4384-9066-504BBC3028C9}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,10 +618,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -608,129 +635,154 @@
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:7" s="7" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G11" r:id="rId1" xr:uid="{47AD0217-7E5D-4F84-AFDF-1906B626308D}"/>
@@ -738,12 +790,19 @@
     <hyperlink ref="G14" r:id="rId3" xr:uid="{619A18E6-8118-463F-828E-2A8E7EF85004}"/>
     <hyperlink ref="G5" r:id="rId4" xr:uid="{AA3E8FE2-2284-4E2B-8970-456561DE2C2F}"/>
     <hyperlink ref="G8" r:id="rId5" xr:uid="{0498A5F7-0BB6-49B4-9608-BFD730565CBC}"/>
+    <hyperlink ref="G17" r:id="rId6" xr:uid="{9B71D05A-3038-4DB7-BA45-D4249188B72B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B4D70A9ADD8C5943AD7F5CA9BE2666A9" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9a3d9ed46e35dd80e2d6c6a9063cb7de">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cb17fdf2-7fd7-4f2e-a077-c317d1fc48a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3a4636362a1cb8f8db250fe9836cbf22" ns3:_="">
     <xsd:import namespace="cb17fdf2-7fd7-4f2e-a077-c317d1fc48a1"/>
@@ -875,7 +934,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -884,13 +943,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93866DF7-5DF0-4FC7-9147-551F8BBBBD36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="cb17fdf2-7fd7-4f2e-a077-c317d1fc48a1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF61E994-8A4D-41F3-AF0B-208217CC2D65}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -908,26 +977,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA659587-CCCD-44D4-A7CF-A2BCB8B789B7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93866DF7-5DF0-4FC7-9147-551F8BBBBD36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="cb17fdf2-7fd7-4f2e-a077-c317d1fc48a1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>